<commit_message>
Tentativo poco riuscito con stan
</commit_message>
<xml_diff>
--- a/dati_2023/01.xlsx
+++ b/dati_2023/01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\R\elezioni\dati_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9B9CB1-6163-463F-B07D-FBB22AAB22CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235B15A9-8934-48B0-8450-E32A522CBFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>LISTA</t>
   </si>
@@ -131,6 +131,15 @@
   </si>
   <si>
     <t>Europa Verde - Sinistra Italiana</t>
+  </si>
+  <si>
+    <t>AREA</t>
+  </si>
+  <si>
+    <t>CENTRO</t>
+  </si>
+  <si>
+    <t>SX-VERDI</t>
   </si>
 </sst>
 </file>
@@ -462,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +488,7 @@
     <col min="7" max="7" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -507,8 +516,11 @@
       <c r="I1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -536,8 +548,11 @@
       <c r="I2">
         <v>240</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -565,8 +580,11 @@
       <c r="I3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -594,8 +612,11 @@
       <c r="I4">
         <v>210</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -623,8 +644,11 @@
       <c r="I5">
         <v>180</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -652,8 +676,11 @@
       <c r="I6">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -681,8 +708,11 @@
       <c r="I7">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -710,8 +740,11 @@
       <c r="I8">
         <v>300</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -736,8 +769,11 @@
       <c r="I9">
         <v>270</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -765,8 +801,11 @@
       <c r="I10">
         <v>120</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -786,7 +825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -806,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -826,7 +865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -846,7 +885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Simulazione basata sui dati passati locali
</commit_message>
<xml_diff>
--- a/dati_2023/01.xlsx
+++ b/dati_2023/01.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\R\elezioni\dati_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235B15A9-8934-48B0-8450-E32A522CBFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA06F6FD-202D-4C53-9951-D08858399724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="liste_naz" sheetId="1" r:id="rId1"/>
+    <sheet name="altri_dati" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>LISTA</t>
   </si>
@@ -79,21 +80,6 @@
     <t>SX</t>
   </si>
   <si>
-    <t>Altro 1</t>
-  </si>
-  <si>
-    <t>Altro 2</t>
-  </si>
-  <si>
-    <t>Altro 3</t>
-  </si>
-  <si>
-    <t>Altro 4</t>
-  </si>
-  <si>
-    <t>Altro 5</t>
-  </si>
-  <si>
     <t>FRAZ_UNI</t>
   </si>
   <si>
@@ -124,9 +110,6 @@
     <t>IV</t>
   </si>
   <si>
-    <t>EV-SI</t>
-  </si>
-  <si>
     <t>ABBREV</t>
   </si>
   <si>
@@ -140,6 +123,18 @@
   </si>
   <si>
     <t>SX-VERDI</t>
+  </si>
+  <si>
+    <t>Art. 1 - MDP</t>
+  </si>
+  <si>
+    <t>MDP</t>
+  </si>
+  <si>
+    <t>Astensione</t>
+  </si>
+  <si>
+    <t>EV - SI</t>
   </si>
 </sst>
 </file>
@@ -471,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +488,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -505,19 +500,19 @@
         <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -525,10 +520,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1">
-        <v>0.23300000000000001</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -557,10 +552,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1">
-        <v>0.22800000000000001</v>
+        <v>0.218</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -581,7 +576,7 @@
         <v>30</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -592,7 +587,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1">
-        <v>0.14699999999999999</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -621,10 +616,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1">
-        <v>0.1</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -653,10 +648,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1">
-        <v>9.4E-2</v>
+        <v>0.107</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -677,7 +672,7 @@
         <v>60</v>
       </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -685,10 +680,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1">
-        <v>5.1999999999999998E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -709,7 +704,7 @@
         <v>45</v>
       </c>
       <c r="J7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -717,10 +712,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1">
-        <v>2.9000000000000001E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -741,7 +736,7 @@
         <v>300</v>
       </c>
       <c r="J8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -775,13 +770,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -802,15 +797,21 @@
         <v>120</v>
       </c>
       <c r="J10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
       </c>
       <c r="C11" s="1">
-        <v>0.01</v>
+        <v>1.9E-2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -824,85 +825,39 @@
       <c r="H11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="I11">
         <v>15</v>
       </c>
-      <c r="C12" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-      <c r="H12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1.6E-2</v>
-      </c>
-      <c r="E15" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1.6E-2</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" t="b">
-        <v>0</v>
+      <c r="J11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B377E1-7781-4663-9DCF-54833628D47E}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corretto numero di senatori per il Molise
</commit_message>
<xml_diff>
--- a/dati_2023/01.xlsx
+++ b/dati_2023/01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\R\elezioni\dati_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA06F6FD-202D-4C53-9951-D08858399724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404D8311-6C0A-4E26-8739-1BD6FBED7DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="liste_naz" sheetId="1" r:id="rId1"/>
@@ -181,10 +181,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -466,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="K11" sqref="K1:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +484,7 @@
     <col min="7" max="7" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +516,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -546,8 +547,9 @@
       <c r="J2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -578,8 +580,9 @@
       <c r="J3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -610,8 +613,9 @@
       <c r="J4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -642,8 +646,9 @@
       <c r="J5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -674,8 +679,9 @@
       <c r="J6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -706,8 +712,9 @@
       <c r="J7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -738,8 +745,9 @@
       <c r="J8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -767,8 +775,9 @@
       <c r="J9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -799,8 +808,9 @@
       <c r="J10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -831,6 +841,7 @@
       <c r="J11" t="s">
         <v>27</v>
       </c>
+      <c r="K11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Inizio migrazione a RMarkdown
</commit_message>
<xml_diff>
--- a/dati_2023/01.xlsx
+++ b/dati_2023/01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\R\elezioni\dati_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FBD0D3-C38B-417F-9BAF-AB50A2D917A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076E52B0-8EF3-4C13-A892-2E0E182BDC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="liste_naz" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>LISTA</t>
   </si>
@@ -137,10 +137,31 @@
     <t>EV - SI</t>
   </si>
   <si>
-    <t>Altri di cdx</t>
-  </si>
-  <si>
-    <t>Insieme per il futuro</t>
+    <t>Noi con l'Italia</t>
+  </si>
+  <si>
+    <t>Altri 1</t>
+  </si>
+  <si>
+    <t>Altri 2</t>
+  </si>
+  <si>
+    <t>Altri 3</t>
+  </si>
+  <si>
+    <t>Altri 4</t>
+  </si>
+  <si>
+    <t>Altri 5</t>
+  </si>
+  <si>
+    <t>ALTRI</t>
+  </si>
+  <si>
+    <t>Sondaggio</t>
+  </si>
+  <si>
+    <t>SWG 18/7/22</t>
   </si>
 </sst>
 </file>
@@ -473,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +551,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1">
-        <v>0.22700000000000001</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -539,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>0.22700000000000001</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="G2" s="2">
         <v>0.26</v>
@@ -563,7 +584,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1">
-        <v>0.218</v>
+        <v>0.221</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -572,7 +593,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>0.218</v>
+        <v>0.221</v>
       </c>
       <c r="G3" s="2">
         <v>0.3</v>
@@ -596,7 +617,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1">
-        <v>0.152</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -605,7 +626,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>0.152</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G4" s="2">
         <v>0.32</v>
@@ -629,7 +650,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="1">
-        <v>0.114</v>
+        <v>0.112</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -638,7 +659,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <v>0.114</v>
+        <v>0.112</v>
       </c>
       <c r="G5" s="2">
         <v>0.23</v>
@@ -662,7 +683,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -671,7 +692,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="G6" s="2">
         <v>0.28000000000000003</v>
@@ -695,7 +716,7 @@
         <v>22</v>
       </c>
       <c r="C7" s="1">
-        <v>4.8000000000000001E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -704,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="1">
-        <v>4.8000000000000001E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="G7" s="2">
         <v>0.4</v>
@@ -728,7 +749,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="1">
-        <v>0.04</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -737,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <v>0.04</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="G8" s="2">
         <v>0.4</v>
@@ -761,7 +782,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -770,7 +791,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="G9" s="2">
         <v>0.35</v>
@@ -794,13 +815,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="1">
-        <v>2.3E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
       </c>
       <c r="F10" s="1">
-        <v>2.3E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="G10" s="2">
         <v>0.35</v>
@@ -824,7 +845,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="1">
-        <v>1.4E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -833,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="1">
-        <v>1.4E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="G11" s="2">
         <v>0.4</v>
@@ -854,7 +875,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="1">
-        <v>1.0999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -863,13 +884,16 @@
         <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>1.0999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="G12" s="2">
         <v>0.3</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
+      </c>
+      <c r="I12">
+        <v>202</v>
       </c>
       <c r="J12" t="s">
         <v>12</v>
@@ -880,16 +904,13 @@
         <v>34</v>
       </c>
       <c r="C13" s="1">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
+        <v>0.01</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
       </c>
       <c r="F13" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="G13" s="2">
         <v>0.25</v>
@@ -898,7 +919,99 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>21</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -911,25 +1024,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B377E1-7781-4663-9DCF-54833628D47E}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>0.5</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix pluricandidature nello stesso collegio
</commit_message>
<xml_diff>
--- a/dati_2023/01.xlsx
+++ b/dati_2023/01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\R\elezioni\dati_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076E52B0-8EF3-4C13-A892-2E0E182BDC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDB000B-4A89-4B80-A0D3-66556BB68070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="liste_naz" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>LISTA</t>
   </si>
@@ -137,9 +137,6 @@
     <t>EV - SI</t>
   </si>
   <si>
-    <t>Noi con l'Italia</t>
-  </si>
-  <si>
     <t>Altri 1</t>
   </si>
   <si>
@@ -161,7 +158,16 @@
     <t>Sondaggio</t>
   </si>
   <si>
-    <t>SWG 18/7/22</t>
+    <t>Insieme per il futuro</t>
+  </si>
+  <si>
+    <t>IxF</t>
+  </si>
+  <si>
+    <t>Altri 6</t>
+  </si>
+  <si>
+    <t>Youtrend per Sky TG24 25/7</t>
   </si>
 </sst>
 </file>
@@ -494,9 +500,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -584,7 +590,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1">
-        <v>0.221</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -593,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>0.221</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="G3" s="2">
         <v>0.3</v>
@@ -617,7 +623,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1">
-        <v>0.14000000000000001</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -626,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>0.14000000000000001</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="G4" s="2">
         <v>0.32</v>
@@ -650,7 +656,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="1">
-        <v>0.112</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -659,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <v>0.112</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="G5" s="2">
         <v>0.23</v>
@@ -683,7 +689,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="1">
-        <v>7.3999999999999996E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -692,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>7.3999999999999996E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="G6" s="2">
         <v>0.28000000000000003</v>
@@ -749,7 +755,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="1">
-        <v>3.7999999999999999E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -758,7 +764,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <v>3.7999999999999999E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="G8" s="2">
         <v>0.4</v>
@@ -776,13 +782,13 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C9" s="1">
-        <v>2.7E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -791,37 +797,40 @@
         <v>0</v>
       </c>
       <c r="F9" s="1">
-        <v>2.7E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="G9" s="2">
-        <v>0.35</v>
+        <v>0.23</v>
       </c>
       <c r="H9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>300</v>
+        <v>55</v>
       </c>
       <c r="J9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
       </c>
       <c r="F10" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="G10" s="2">
         <v>0.35</v>
@@ -830,78 +839,79 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="J10" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
-        <v>2.3E-2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>13</v>
+        <v>0.02</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
       <c r="F11" s="1">
-        <v>2.3E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G11" s="2">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>15</v>
+        <v>270</v>
       </c>
       <c r="J11" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
       </c>
       <c r="C12" s="1">
-        <v>0.01</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>0.01</v>
+        <v>1.6E-2</v>
       </c>
       <c r="G12" s="2">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>202</v>
+        <v>15</v>
       </c>
       <c r="J12" t="s">
-        <v>12</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1">
         <v>0.01</v>
@@ -919,12 +929,12 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1">
         <v>0.01</v>
@@ -942,12 +952,12 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1">
         <v>0.01</v>
@@ -965,12 +975,12 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="1">
         <v>0.01</v>
@@ -988,21 +998,21 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1">
-        <v>3.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
       </c>
       <c r="F17" s="1">
-        <v>3.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="G17" s="2">
         <v>0.25</v>
@@ -1011,7 +1021,30 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1026,19 +1059,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B377E1-7781-4663-9DCF-54833628D47E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>31</v>
@@ -1046,10 +1079,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2">
-        <v>0.43</v>
+        <v>0.41699999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mediana anziché media, e precedenti modifiche.
</commit_message>
<xml_diff>
--- a/dati_2023/01.xlsx
+++ b/dati_2023/01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\R\elezioni\dati_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDB000B-4A89-4B80-A0D3-66556BB68070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C564F2-7535-4E18-B6F7-C9A3120EE377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="liste_naz" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>LISTA</t>
   </si>
@@ -77,9 +77,6 @@
     <t>DX</t>
   </si>
   <si>
-    <t>SX</t>
-  </si>
-  <si>
     <t>FRAZ_UNI</t>
   </si>
   <si>
@@ -125,21 +122,12 @@
     <t>SX-VERDI</t>
   </si>
   <si>
-    <t>Art. 1 - MDP</t>
-  </si>
-  <si>
-    <t>MDP</t>
-  </si>
-  <si>
     <t>Astensione</t>
   </si>
   <si>
     <t>EV - SI</t>
   </si>
   <si>
-    <t>Altri 1</t>
-  </si>
-  <si>
     <t>Altri 2</t>
   </si>
   <si>
@@ -158,16 +146,28 @@
     <t>Sondaggio</t>
   </si>
   <si>
-    <t>Insieme per il futuro</t>
-  </si>
-  <si>
-    <t>IxF</t>
-  </si>
-  <si>
-    <t>Altri 6</t>
-  </si>
-  <si>
-    <t>Youtrend per Sky TG24 25/7</t>
+    <t>Impegno civico</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>Alternativa per l'Italia</t>
+  </si>
+  <si>
+    <t>ApI</t>
+  </si>
+  <si>
+    <t>Italia Sovrana e Popolare</t>
+  </si>
+  <si>
+    <t>ISP</t>
+  </si>
+  <si>
+    <t>BiDiMedia 5 ago</t>
+  </si>
+  <si>
+    <t>CSX</t>
   </si>
 </sst>
 </file>
@@ -214,11 +214,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -500,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="F2" sqref="F2:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -534,19 +535,19 @@
         <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
       <c r="J1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -554,10 +555,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1">
-        <v>0.23799999999999999</v>
+        <v>0.245</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -566,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>0.23799999999999999</v>
+        <v>0.245</v>
       </c>
       <c r="G2" s="2">
         <v>0.26</v>
@@ -587,19 +588,19 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1">
-        <v>0.22500000000000001</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>0.22500000000000001</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="G3" s="2">
         <v>0.3</v>
@@ -611,7 +612,7 @@
         <v>30</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K3" s="3"/>
     </row>
@@ -623,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1">
-        <v>0.13400000000000001</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -632,7 +633,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>0.13400000000000001</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="G4" s="2">
         <v>0.32</v>
@@ -653,19 +654,16 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <v>9.8000000000000004E-2</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="G5" s="2">
         <v>0.23</v>
@@ -677,7 +675,7 @@
         <v>60</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K5" s="3"/>
     </row>
@@ -686,10 +684,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1">
-        <v>8.3000000000000004E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -698,7 +696,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>8.3000000000000004E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="G6" s="2">
         <v>0.28000000000000003</v>
@@ -719,19 +717,19 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1">
-        <v>4.9000000000000002E-2</v>
+        <v>0.06</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
       <c r="F7" s="1">
-        <v>4.9000000000000002E-2</v>
+        <v>0.06</v>
       </c>
       <c r="G7" s="2">
         <v>0.4</v>
@@ -743,28 +741,28 @@
         <v>45</v>
       </c>
       <c r="J7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="G8" s="2">
         <v>0.4</v>
@@ -776,40 +774,37 @@
         <v>120</v>
       </c>
       <c r="J8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
+        <v>2.3E-2</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
       </c>
       <c r="F9" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="G9" s="2">
-        <v>0.23</v>
+        <v>0.35</v>
       </c>
       <c r="H9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>55</v>
+        <v>270</v>
       </c>
       <c r="J9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="K9" s="3"/>
     </row>
@@ -818,19 +813,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
+        <v>0.02</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
       </c>
       <c r="F10" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G10" s="2">
         <v>0.35</v>
@@ -842,34 +834,34 @@
         <v>300</v>
       </c>
       <c r="J10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
       <c r="F11" s="1">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="G11" s="2">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="J11" t="s">
         <v>12</v>
@@ -878,49 +870,52 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1">
-        <v>1.6E-2</v>
+        <v>0.01</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>1.6E-2</v>
+        <v>0.01</v>
       </c>
       <c r="G12" s="2">
-        <v>0.4</v>
+        <v>0.23</v>
       </c>
       <c r="H12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="J12" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
       </c>
       <c r="C13" s="1">
-        <v>0.01</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
       </c>
       <c r="F13" s="1">
-        <v>0.01</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="G13" s="2">
         <v>0.25</v>
@@ -928,13 +923,17 @@
       <c r="H13" t="b">
         <v>0</v>
       </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
       <c r="J13" t="s">
-        <v>38</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1">
         <v>0.01</v>
@@ -952,12 +951,12 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1">
         <v>0.01</v>
@@ -975,12 +974,12 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1">
         <v>0.01</v>
@@ -998,12 +997,12 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C17" s="1">
         <v>0.01</v>
@@ -1021,35 +1020,15 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="E18" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="H18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
-        <v>38</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F19" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J13">
-    <sortCondition descending="1" ref="C2:C13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J18">
+    <sortCondition descending="1" ref="C2:C18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1060,7 +1039,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,21 +1050,22 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>43</v>
+      <c r="A2" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="2">
-        <v>0.41699999999999998</v>
+        <v>0.375</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>